<commit_message>
Update Leave Card 3/17/2023 4:42 PM
</commit_message>
<xml_diff>
--- a/DONE/MULINGTAPANG, GUILLERMA.xlsx
+++ b/DONE/MULINGTAPANG, GUILLERMA.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DESKTOP-44REB32\Users\ASUS\Desktop\LEAVECARD\DONE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVECARD\DONE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE83EF4B-4EC6-4F80-960D-601D23364744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2018 LEAVE CREDITS" sheetId="4" r:id="rId1"/>
@@ -26,25 +27,17 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2017 LEAVE BALANCE'!$1:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'2018 LEAVE CREDITS'!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
   <si>
     <t>PERIOD</t>
   </si>
@@ -229,7 +222,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -608,17 +601,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -628,6 +618,9 @@
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1156,25 +1149,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A8:K128" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A8:K128" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="11">
-    <tableColumn id="1" name="PERIOD" dataDxfId="25"/>
-    <tableColumn id="2" name="PARTICULARS" dataDxfId="24"/>
-    <tableColumn id="3" name="EARNED" dataDxfId="23"/>
-    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="22"/>
-    <tableColumn id="5" name="BALANCE" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EARNED" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BALANCE" dataDxfId="21">
       <calculatedColumnFormula>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="20"/>
-    <tableColumn id="7" name="EARNED " dataDxfId="19">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EARNED " dataDxfId="19">
       <calculatedColumnFormula>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
-    <tableColumn id="9" name="BALANCE " dataDxfId="17">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BALANCE " dataDxfId="17">
       <calculatedColumnFormula>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
-    <tableColumn id="11" name="REMARKS" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="REMARKS" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1186,25 +1179,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K68" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A8:K68" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
-    <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
-    <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
-    <tableColumn id="3" name="EARNED" dataDxfId="8"/>
-    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="7"/>
-    <tableColumn id="5" name="BALANCE" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="PERIOD" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PARTICULARS" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="EARNED" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="BALANCE" dataDxfId="6">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="5"/>
-    <tableColumn id="7" name="EARNED " dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="EARNED " dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
-    <tableColumn id="9" name="BALANCE " dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BALANCE " dataDxfId="2">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
-    <tableColumn id="11" name="REMARKS" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="REMARKS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1511,34 +1504,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A58" activePane="bottomLeft"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3696" topLeftCell="A70" activePane="bottomLeft"/>
       <selection activeCell="B4" sqref="B4:C4"/>
-      <selection pane="bottomLeft" activeCell="B76" sqref="B76"/>
+      <selection pane="bottomLeft" activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -1550,16 +1543,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -1568,18 +1561,18 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="55">
+      <c r="F3" s="54">
         <v>42552</v>
       </c>
-      <c r="G3" s="51"/>
+      <c r="G3" s="52"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="57"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -1590,16 +1583,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="52"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="52"/>
+      <c r="K4" s="53"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -1607,7 +1600,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -1620,24 +1613,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53" t="s">
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -1672,7 +1665,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -1696,7 +1689,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="48" t="s">
         <v>44</v>
       </c>
@@ -1718,7 +1711,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="40">
         <v>43101</v>
       </c>
@@ -1738,7 +1731,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="40">
         <v>43132</v>
       </c>
@@ -1758,7 +1751,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="40">
         <v>43160</v>
       </c>
@@ -1778,7 +1771,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="40">
         <v>43191</v>
       </c>
@@ -1798,7 +1791,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="40">
         <v>43221</v>
       </c>
@@ -1818,7 +1811,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="40">
         <v>43252</v>
       </c>
@@ -1838,7 +1831,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="40">
         <v>43282</v>
       </c>
@@ -1858,7 +1851,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="40">
         <v>43313</v>
       </c>
@@ -1878,7 +1871,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="40">
         <v>43344</v>
       </c>
@@ -1898,7 +1891,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="40">
         <v>43374</v>
       </c>
@@ -1918,7 +1911,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="40">
         <v>43405</v>
       </c>
@@ -1938,7 +1931,7 @@
       <c r="J21" s="11"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="40">
         <v>43435</v>
       </c>
@@ -1962,7 +1955,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="48" t="s">
         <v>45</v>
       </c>
@@ -1980,7 +1973,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="40">
         <v>43466</v>
       </c>
@@ -2000,7 +1993,7 @@
       <c r="J24" s="11"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="40">
         <v>43497</v>
       </c>
@@ -2020,7 +2013,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="40">
         <v>43525</v>
       </c>
@@ -2040,7 +2033,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="40">
         <v>43556</v>
       </c>
@@ -2060,7 +2053,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="40">
         <v>43586</v>
       </c>
@@ -2080,7 +2073,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="40">
         <v>43617</v>
       </c>
@@ -2100,7 +2093,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="40">
         <v>43647</v>
       </c>
@@ -2120,7 +2113,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="40">
         <v>43678</v>
       </c>
@@ -2140,7 +2133,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="40">
         <v>43709</v>
       </c>
@@ -2160,7 +2153,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="40">
         <v>43739</v>
       </c>
@@ -2180,7 +2173,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="40">
         <v>43770</v>
       </c>
@@ -2200,7 +2193,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="40">
         <v>43800</v>
       </c>
@@ -2224,7 +2217,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="48" t="s">
         <v>46</v>
       </c>
@@ -2242,7 +2235,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="40">
         <v>43831</v>
       </c>
@@ -2262,7 +2255,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="40">
         <v>43862</v>
       </c>
@@ -2282,7 +2275,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="40">
         <v>43891</v>
       </c>
@@ -2302,7 +2295,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="40">
         <v>43922</v>
       </c>
@@ -2322,7 +2315,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="40">
         <v>43952</v>
       </c>
@@ -2342,7 +2335,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="40">
         <v>43983</v>
       </c>
@@ -2362,7 +2355,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="40">
         <v>44013</v>
       </c>
@@ -2382,7 +2375,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="40">
         <v>44044</v>
       </c>
@@ -2402,7 +2395,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="40">
         <v>44075</v>
       </c>
@@ -2422,7 +2415,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="40">
         <v>44105</v>
       </c>
@@ -2442,7 +2435,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="40">
         <v>44136</v>
       </c>
@@ -2462,7 +2455,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="40">
         <v>44166</v>
       </c>
@@ -2486,7 +2479,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="48" t="s">
         <v>47</v>
       </c>
@@ -2504,7 +2497,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="40">
         <v>44197</v>
       </c>
@@ -2524,7 +2517,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="40">
         <v>44228</v>
       </c>
@@ -2544,7 +2537,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="40">
         <v>44256</v>
       </c>
@@ -2564,7 +2557,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="40">
         <v>44287</v>
       </c>
@@ -2584,7 +2577,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="40">
         <v>44317</v>
       </c>
@@ -2604,7 +2597,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="40">
         <v>44348</v>
       </c>
@@ -2624,7 +2617,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="40">
         <v>44378</v>
       </c>
@@ -2644,7 +2637,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="40">
         <v>44409</v>
       </c>
@@ -2664,7 +2657,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="40">
         <v>44440</v>
       </c>
@@ -2684,7 +2677,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="40">
         <v>44470</v>
       </c>
@@ -2704,7 +2697,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="40">
         <v>44501</v>
       </c>
@@ -2724,7 +2717,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="40">
         <v>44531</v>
       </c>
@@ -2748,7 +2741,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="48" t="s">
         <v>48</v>
       </c>
@@ -2766,7 +2759,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="40">
         <v>44562</v>
       </c>
@@ -2786,7 +2779,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="40">
         <v>44593</v>
       </c>
@@ -2806,7 +2799,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="40">
         <v>44621</v>
       </c>
@@ -2826,7 +2819,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="40">
         <v>44652</v>
       </c>
@@ -2846,7 +2839,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="40">
         <v>44682</v>
       </c>
@@ -2866,7 +2859,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="40">
         <v>44713</v>
       </c>
@@ -2886,7 +2879,7 @@
       <c r="J68" s="11"/>
       <c r="K68" s="49"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="40">
         <v>44743</v>
       </c>
@@ -2906,7 +2899,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="40">
         <v>44774</v>
       </c>
@@ -2932,7 +2925,7 @@
         <v>44803</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="40">
         <v>44805</v>
       </c>
@@ -2952,7 +2945,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="40">
         <v>44835</v>
       </c>
@@ -2972,7 +2965,7 @@
       <c r="J72" s="11"/>
       <c r="K72" s="49"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="40">
         <v>44866</v>
       </c>
@@ -2998,7 +2991,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="40">
         <v>44896</v>
       </c>
@@ -3024,7 +3017,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="48" t="s">
         <v>59</v>
       </c>
@@ -3042,7 +3035,7 @@
       <c r="J75" s="11"/>
       <c r="K75" s="20"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="40">
         <v>44927</v>
       </c>
@@ -3062,7 +3055,7 @@
       <c r="J76" s="11"/>
       <c r="K76" s="20"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="40">
         <v>44958</v>
       </c>
@@ -3082,7 +3075,7 @@
       <c r="J77" s="11"/>
       <c r="K77" s="20"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="40"/>
       <c r="B78" s="20"/>
       <c r="C78" s="13"/>
@@ -3098,7 +3091,7 @@
       <c r="J78" s="11"/>
       <c r="K78" s="20"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="40"/>
       <c r="B79" s="20"/>
       <c r="C79" s="13"/>
@@ -3114,7 +3107,7 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="40"/>
       <c r="B80" s="20"/>
       <c r="C80" s="13"/>
@@ -3130,7 +3123,7 @@
       <c r="J80" s="11"/>
       <c r="K80" s="20"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="40"/>
       <c r="B81" s="20"/>
       <c r="C81" s="13"/>
@@ -3146,7 +3139,7 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="40"/>
       <c r="B82" s="20"/>
       <c r="C82" s="13"/>
@@ -3162,7 +3155,7 @@
       <c r="J82" s="11"/>
       <c r="K82" s="20"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="40"/>
       <c r="B83" s="20"/>
       <c r="C83" s="13"/>
@@ -3178,7 +3171,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="40"/>
       <c r="B84" s="20"/>
       <c r="C84" s="13"/>
@@ -3194,7 +3187,7 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="40"/>
       <c r="B85" s="20"/>
       <c r="C85" s="13"/>
@@ -3210,7 +3203,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="40"/>
       <c r="B86" s="20"/>
       <c r="C86" s="13"/>
@@ -3226,7 +3219,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="40"/>
       <c r="B87" s="20"/>
       <c r="C87" s="13"/>
@@ -3242,7 +3235,7 @@
       <c r="J87" s="11"/>
       <c r="K87" s="20"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="40"/>
       <c r="B88" s="20"/>
       <c r="C88" s="13"/>
@@ -3258,7 +3251,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="40"/>
       <c r="B89" s="20"/>
       <c r="C89" s="13"/>
@@ -3274,7 +3267,7 @@
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="40"/>
       <c r="B90" s="20"/>
       <c r="C90" s="13"/>
@@ -3290,7 +3283,7 @@
       <c r="J90" s="11"/>
       <c r="K90" s="20"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="40"/>
       <c r="B91" s="20"/>
       <c r="C91" s="13"/>
@@ -3306,7 +3299,7 @@
       <c r="J91" s="11"/>
       <c r="K91" s="20"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="40"/>
       <c r="B92" s="20"/>
       <c r="C92" s="13"/>
@@ -3322,7 +3315,7 @@
       <c r="J92" s="11"/>
       <c r="K92" s="20"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="40"/>
       <c r="B93" s="20"/>
       <c r="C93" s="13"/>
@@ -3338,7 +3331,7 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="40"/>
       <c r="B94" s="20"/>
       <c r="C94" s="13"/>
@@ -3354,7 +3347,7 @@
       <c r="J94" s="11"/>
       <c r="K94" s="20"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="40"/>
       <c r="B95" s="20"/>
       <c r="C95" s="13"/>
@@ -3370,7 +3363,7 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="40"/>
       <c r="B96" s="20"/>
       <c r="C96" s="13"/>
@@ -3386,7 +3379,7 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="40"/>
       <c r="B97" s="20"/>
       <c r="C97" s="13"/>
@@ -3402,7 +3395,7 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="40"/>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
@@ -3418,7 +3411,7 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="40"/>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
@@ -3434,7 +3427,7 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="40"/>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
@@ -3450,7 +3443,7 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="40"/>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
@@ -3466,7 +3459,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="40"/>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -3482,7 +3475,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="40"/>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -3498,7 +3491,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="40"/>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -3514,7 +3507,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="40"/>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -3530,7 +3523,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="40"/>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -3546,7 +3539,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="40"/>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -3562,7 +3555,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="40"/>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -3578,7 +3571,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="40"/>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -3594,7 +3587,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="40"/>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -3610,7 +3603,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="40"/>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -3626,7 +3619,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="40"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -3642,7 +3635,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="40"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -3658,7 +3651,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="40"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -3674,7 +3667,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="40"/>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -3690,7 +3683,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="40"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -3706,7 +3699,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="40"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -3722,7 +3715,7 @@
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="40"/>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -3738,7 +3731,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="40"/>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -3754,7 +3747,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="40"/>
       <c r="B120" s="20"/>
       <c r="C120" s="13"/>
@@ -3770,7 +3763,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="40"/>
       <c r="B121" s="20"/>
       <c r="C121" s="13"/>
@@ -3786,7 +3779,7 @@
       <c r="J121" s="11"/>
       <c r="K121" s="20"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" s="40"/>
       <c r="B122" s="20"/>
       <c r="C122" s="13"/>
@@ -3802,7 +3795,7 @@
       <c r="J122" s="11"/>
       <c r="K122" s="20"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="40"/>
       <c r="B123" s="20"/>
       <c r="C123" s="13"/>
@@ -3818,7 +3811,7 @@
       <c r="J123" s="11"/>
       <c r="K123" s="20"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="40"/>
       <c r="B124" s="20"/>
       <c r="C124" s="13"/>
@@ -3834,7 +3827,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" s="40"/>
       <c r="B125" s="20"/>
       <c r="C125" s="13"/>
@@ -3850,7 +3843,7 @@
       <c r="J125" s="11"/>
       <c r="K125" s="20"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" s="40"/>
       <c r="B126" s="20"/>
       <c r="C126" s="13"/>
@@ -3866,7 +3859,7 @@
       <c r="J126" s="11"/>
       <c r="K126" s="20"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" s="40"/>
       <c r="B127" s="20"/>
       <c r="C127" s="13"/>
@@ -3882,7 +3875,7 @@
       <c r="J127" s="11"/>
       <c r="K127" s="20"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" s="41"/>
       <c r="B128" s="15"/>
       <c r="C128" s="42"/>
@@ -3900,23 +3893,23 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3939,34 +3932,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K68"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A7" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3696" topLeftCell="A7" activePane="bottomLeft"/>
       <selection activeCell="B4" sqref="B4:C4"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -3978,16 +3971,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -3996,18 +3989,18 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="55">
+      <c r="F3" s="54">
         <v>42552</v>
       </c>
-      <c r="G3" s="51"/>
+      <c r="G3" s="52"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="57"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -4018,16 +4011,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="52"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="52"/>
+      <c r="K4" s="53"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -4035,7 +4028,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -4048,24 +4041,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53" t="s">
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -4100,7 +4093,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -4119,12 +4112,12 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
-        <v>61.5</v>
+        <v>60.5</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="48" t="s">
         <v>48</v>
       </c>
@@ -4142,7 +4135,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="40">
         <v>44713</v>
       </c>
@@ -4166,7 +4159,7 @@
         <v>44740</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="40">
         <v>44774</v>
       </c>
@@ -4190,7 +4183,7 @@
         <v>44797</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="40">
         <v>44835</v>
       </c>
@@ -4212,7 +4205,7 @@
         <v>44860</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="40"/>
       <c r="B14" s="20" t="s">
         <v>52</v>
@@ -4234,8 +4227,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="48" t="s">
+        <v>59</v>
+      </c>
       <c r="B15" s="20"/>
       <c r="C15" s="13"/>
       <c r="D15" s="39"/>
@@ -4250,9 +4245,13 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="20"/>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="40">
+        <v>44945</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>49</v>
+      </c>
       <c r="C16" s="13"/>
       <c r="D16" s="39"/>
       <c r="E16" s="9"/>
@@ -4261,12 +4260,16 @@
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H16" s="39"/>
+      <c r="H16" s="39">
+        <v>1</v>
+      </c>
       <c r="I16" s="9"/>
       <c r="J16" s="11"/>
-      <c r="K16" s="20"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="49">
+        <v>44574</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="40"/>
       <c r="B17" s="20"/>
       <c r="C17" s="13"/>
@@ -4282,7 +4285,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="40"/>
       <c r="B18" s="20"/>
       <c r="C18" s="13"/>
@@ -4298,7 +4301,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="40"/>
       <c r="B19" s="20"/>
       <c r="C19" s="13"/>
@@ -4314,7 +4317,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="40"/>
       <c r="B20" s="20"/>
       <c r="C20" s="13"/>
@@ -4330,7 +4333,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="40"/>
       <c r="B21" s="20"/>
       <c r="C21" s="13"/>
@@ -4346,7 +4349,7 @@
       <c r="J21" s="11"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="40"/>
       <c r="B22" s="20"/>
       <c r="C22" s="13"/>
@@ -4362,7 +4365,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="40"/>
       <c r="B23" s="20"/>
       <c r="C23" s="13"/>
@@ -4378,7 +4381,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="40"/>
       <c r="B24" s="20"/>
       <c r="C24" s="13"/>
@@ -4394,7 +4397,7 @@
       <c r="J24" s="11"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="40"/>
       <c r="B25" s="20"/>
       <c r="C25" s="13"/>
@@ -4410,7 +4413,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="40"/>
       <c r="B26" s="20"/>
       <c r="C26" s="13"/>
@@ -4426,7 +4429,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="40"/>
       <c r="B27" s="20"/>
       <c r="C27" s="13"/>
@@ -4442,7 +4445,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="40"/>
       <c r="B28" s="20"/>
       <c r="C28" s="13"/>
@@ -4458,7 +4461,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="40"/>
       <c r="B29" s="20"/>
       <c r="C29" s="13"/>
@@ -4474,7 +4477,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="40"/>
       <c r="B30" s="20"/>
       <c r="C30" s="13"/>
@@ -4490,7 +4493,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="40"/>
       <c r="B31" s="20"/>
       <c r="C31" s="13"/>
@@ -4506,7 +4509,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="40"/>
       <c r="B32" s="20"/>
       <c r="C32" s="13"/>
@@ -4522,7 +4525,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="40"/>
       <c r="B33" s="20"/>
       <c r="C33" s="13"/>
@@ -4538,7 +4541,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="40"/>
       <c r="B34" s="20"/>
       <c r="C34" s="13"/>
@@ -4554,7 +4557,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="40"/>
       <c r="B35" s="20"/>
       <c r="C35" s="13"/>
@@ -4570,7 +4573,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="40"/>
       <c r="B36" s="20"/>
       <c r="C36" s="13"/>
@@ -4586,7 +4589,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="40"/>
       <c r="B37" s="20"/>
       <c r="C37" s="13"/>
@@ -4602,7 +4605,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="40"/>
       <c r="B38" s="20"/>
       <c r="C38" s="13"/>
@@ -4618,7 +4621,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="40"/>
       <c r="B39" s="20"/>
       <c r="C39" s="13"/>
@@ -4634,7 +4637,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="40"/>
       <c r="B40" s="20"/>
       <c r="C40" s="13"/>
@@ -4650,7 +4653,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="40"/>
       <c r="B41" s="20"/>
       <c r="C41" s="13"/>
@@ -4666,7 +4669,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="40"/>
       <c r="B42" s="20"/>
       <c r="C42" s="13"/>
@@ -4682,7 +4685,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="40"/>
       <c r="B43" s="20"/>
       <c r="C43" s="13"/>
@@ -4698,7 +4701,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="40"/>
       <c r="B44" s="20"/>
       <c r="C44" s="13"/>
@@ -4714,7 +4717,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="40"/>
       <c r="B45" s="20"/>
       <c r="C45" s="13"/>
@@ -4730,7 +4733,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="40"/>
       <c r="B46" s="20"/>
       <c r="C46" s="13"/>
@@ -4746,7 +4749,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="40"/>
       <c r="B47" s="20"/>
       <c r="C47" s="13"/>
@@ -4762,7 +4765,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="40"/>
       <c r="B48" s="20"/>
       <c r="C48" s="13"/>
@@ -4778,7 +4781,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="40"/>
       <c r="B49" s="20"/>
       <c r="C49" s="13"/>
@@ -4794,7 +4797,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="40"/>
       <c r="B50" s="20"/>
       <c r="C50" s="13"/>
@@ -4810,7 +4813,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="40"/>
       <c r="B51" s="20"/>
       <c r="C51" s="13"/>
@@ -4826,7 +4829,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="40"/>
       <c r="B52" s="20"/>
       <c r="C52" s="13"/>
@@ -4842,7 +4845,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="40"/>
       <c r="B53" s="20"/>
       <c r="C53" s="13"/>
@@ -4858,7 +4861,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="40"/>
       <c r="B54" s="20"/>
       <c r="C54" s="13"/>
@@ -4874,7 +4877,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="40"/>
       <c r="B55" s="20"/>
       <c r="C55" s="13"/>
@@ -4890,7 +4893,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="40"/>
       <c r="B56" s="20"/>
       <c r="C56" s="13"/>
@@ -4906,7 +4909,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="40"/>
       <c r="B57" s="20"/>
       <c r="C57" s="13"/>
@@ -4922,7 +4925,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="40"/>
       <c r="B58" s="20"/>
       <c r="C58" s="13"/>
@@ -4938,7 +4941,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="40"/>
       <c r="B59" s="20"/>
       <c r="C59" s="13"/>
@@ -4954,7 +4957,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="40"/>
       <c r="B60" s="20"/>
       <c r="C60" s="13"/>
@@ -4970,7 +4973,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="40"/>
       <c r="B61" s="20"/>
       <c r="C61" s="13"/>
@@ -4986,7 +4989,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="40"/>
       <c r="B62" s="20"/>
       <c r="C62" s="13"/>
@@ -5002,7 +5005,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="40"/>
       <c r="B63" s="20"/>
       <c r="C63" s="13"/>
@@ -5018,7 +5021,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="40"/>
       <c r="B64" s="20"/>
       <c r="C64" s="13"/>
@@ -5034,7 +5037,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="40"/>
       <c r="B65" s="20"/>
       <c r="C65" s="13"/>
@@ -5050,7 +5053,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="40"/>
       <c r="B66" s="20"/>
       <c r="C66" s="13"/>
@@ -5066,7 +5069,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="40"/>
       <c r="B67" s="20"/>
       <c r="C67" s="13"/>
@@ -5082,7 +5085,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="41"/>
       <c r="B68" s="15"/>
       <c r="C68" s="42"/>
@@ -5113,10 +5116,10 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5139,28 +5142,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="37" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" style="37" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D1" s="58" t="s">
         <v>33</v>
       </c>
@@ -5173,7 +5176,7 @@
       <c r="K1" s="59"/>
       <c r="L1" s="59"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -5202,7 +5205,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>63.478999999999999</v>
       </c>
@@ -5226,17 +5229,17 @@
         <v>---</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="G4" s="33"/>
       <c r="J4" s="1" t="str">
         <f>IF(TEXT(J3,"D")=1,1,TEXT(J3,"D"))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C6" s="38" t="s">
         <v>28</v>
       </c>
@@ -5257,7 +5260,7 @@
       <c r="K6" s="60"/>
       <c r="L6" s="60"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C7" s="37">
         <v>1</v>
       </c>
@@ -5284,7 +5287,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C8" s="37">
         <v>2</v>
       </c>
@@ -5310,7 +5313,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C9" s="37">
         <v>3</v>
       </c>
@@ -5336,7 +5339,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C10" s="37">
         <v>4</v>
       </c>
@@ -5362,7 +5365,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C11" s="37">
         <v>5</v>
       </c>
@@ -5388,7 +5391,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C12" s="37">
         <v>6</v>
       </c>
@@ -5414,7 +5417,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C13" s="37">
         <v>7</v>
       </c>
@@ -5440,7 +5443,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C14" s="37">
         <v>8</v>
       </c>
@@ -5466,7 +5469,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C15" s="37">
         <v>9</v>
       </c>
@@ -5486,7 +5489,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C16" s="37">
         <v>10</v>
       </c>
@@ -5506,7 +5509,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="37">
         <v>11</v>
       </c>
@@ -5526,7 +5529,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C18" s="37">
         <v>12</v>
       </c>
@@ -5547,7 +5550,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C19" s="37">
         <v>13</v>
       </c>
@@ -5568,7 +5571,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C20" s="37">
         <v>14</v>
       </c>
@@ -5589,7 +5592,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C21" s="37">
         <v>15</v>
       </c>
@@ -5610,7 +5613,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C22" s="37">
         <v>16</v>
       </c>
@@ -5631,7 +5634,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C23" s="37">
         <v>17</v>
       </c>
@@ -5652,7 +5655,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C24" s="37">
         <v>18</v>
       </c>
@@ -5673,7 +5676,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C25" s="37">
         <v>19</v>
       </c>
@@ -5694,7 +5697,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C26" s="37">
         <v>20</v>
       </c>
@@ -5715,7 +5718,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C27" s="37">
         <v>21</v>
       </c>
@@ -5736,7 +5739,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C28" s="37">
         <v>22</v>
       </c>
@@ -5757,7 +5760,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C29" s="37">
         <v>23</v>
       </c>
@@ -5778,7 +5781,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C30" s="37">
         <v>24</v>
       </c>
@@ -5799,7 +5802,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C31" s="37">
         <v>25</v>
       </c>
@@ -5820,7 +5823,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C32" s="37">
         <v>26</v>
       </c>
@@ -5841,7 +5844,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C33" s="37">
         <v>27</v>
       </c>
@@ -5862,7 +5865,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C34" s="37">
         <v>28</v>
       </c>
@@ -5883,7 +5886,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C35" s="37">
         <v>29</v>
       </c>
@@ -5904,7 +5907,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C36" s="37">
         <v>30</v>
       </c>
@@ -5925,7 +5928,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C37" s="37">
         <v>31</v>
       </c>
@@ -5946,7 +5949,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C38" s="37">
         <v>32</v>
       </c>
@@ -5955,7 +5958,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C39" s="37">
         <v>33</v>
       </c>
@@ -5964,7 +5967,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C40" s="37">
         <v>34</v>
       </c>
@@ -5973,7 +5976,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C41" s="37">
         <v>35</v>
       </c>
@@ -5982,7 +5985,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C42" s="37">
         <v>36</v>
       </c>
@@ -5991,7 +5994,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C43" s="37">
         <v>37</v>
       </c>
@@ -6000,7 +6003,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C44" s="37">
         <v>38</v>
       </c>
@@ -6009,7 +6012,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C45" s="37">
         <v>39</v>
       </c>
@@ -6018,7 +6021,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C46" s="37">
         <v>40</v>
       </c>
@@ -6027,7 +6030,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C47" s="37">
         <v>41</v>
       </c>
@@ -6036,7 +6039,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C48" s="37">
         <v>42</v>
       </c>
@@ -6045,7 +6048,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C49" s="37">
         <v>43</v>
       </c>
@@ -6054,7 +6057,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C50" s="37">
         <v>44</v>
       </c>
@@ -6063,7 +6066,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C51" s="37">
         <v>45</v>
       </c>
@@ -6072,7 +6075,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C52" s="37">
         <v>46</v>
       </c>
@@ -6081,7 +6084,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C53" s="37">
         <v>47</v>
       </c>
@@ -6090,7 +6093,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C54" s="37">
         <v>48</v>
       </c>
@@ -6099,7 +6102,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C55" s="37">
         <v>49</v>
       </c>
@@ -6108,7 +6111,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C56" s="37">
         <v>50</v>
       </c>
@@ -6117,7 +6120,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C57" s="37">
         <v>51</v>
       </c>
@@ -6126,7 +6129,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C58" s="37">
         <v>52</v>
       </c>
@@ -6135,7 +6138,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C59" s="37">
         <v>53</v>
       </c>
@@ -6144,7 +6147,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C60" s="37">
         <v>54</v>
       </c>
@@ -6153,7 +6156,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C61" s="37">
         <v>55</v>
       </c>
@@ -6162,7 +6165,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C62" s="37">
         <v>56</v>
       </c>
@@ -6171,7 +6174,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C63" s="37">
         <v>57</v>
       </c>
@@ -6180,7 +6183,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C64" s="37">
         <v>58</v>
       </c>
@@ -6189,7 +6192,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C65" s="37">
         <v>59</v>
       </c>
@@ -6198,7 +6201,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C66" s="37">
         <v>60</v>
       </c>
@@ -6207,7 +6210,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>